<commit_message>
updating readme, adding option to use renv.
</commit_message>
<xml_diff>
--- a/data/metapopulation-inputs.xlsx
+++ b/data/metapopulation-inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plima/dev/genomic-surveillance-voi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2E13B2-5CBC-5C4C-9B03-D36E9F0CC563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71B604B-D3C1-0749-A0F9-EC74F1381ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2900" yWindow="2040" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
+    <workbookView xWindow="2900" yWindow="2040" windowWidth="28040" windowHeight="17440" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="relative-mixing" sheetId="5" r:id="rId4"/>
     <sheet name="parameters" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -496,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D12AAEB-4DB6-F84A-A5FA-6A348965EB1E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1005,7 +1005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930774C7-2D37-094A-A2DB-7EC2D5ACBFA8}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
demonstrating setting inputs from file
</commit_message>
<xml_diff>
--- a/data/metapopulation-inputs.xlsx
+++ b/data/metapopulation-inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plima/dev/genomic-surveillance-voi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71B604B-D3C1-0749-A0F9-EC74F1381ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367237C3-5CEF-C146-B9A3-29DCD4A84D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2900" yWindow="2040" windowWidth="28040" windowHeight="17440" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
+    <workbookView xWindow="2900" yWindow="2040" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>setting</t>
   </si>
@@ -128,6 +128,15 @@
   </si>
   <si>
     <t>distribution</t>
+  </si>
+  <si>
+    <t>jurisdiction</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>source</t>
   </si>
 </sst>
 </file>
@@ -496,7 +505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D12AAEB-4DB6-F84A-A5FA-6A348965EB1E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -646,12 +655,15 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
       <c r="B1" t="str" cm="1">
         <f t="array" ref="B1:G1">TRANSPOSE(A2:A7)</f>
         <v>NY</v>
@@ -826,12 +838,15 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
       <c r="B1" t="str" cm="1">
         <f t="array" ref="B1:G1">TRANSPOSE(A2:A7)</f>
         <v>NY</v>
@@ -1003,15 +1018,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930774C7-2D37-094A-A2DB-7EC2D5ACBFA8}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1027,15 +1042,23 @@
       <c r="E1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating functions and inputs file to accept inputs from spreadsheet
</commit_message>
<xml_diff>
--- a/data/metapopulation-inputs.xlsx
+++ b/data/metapopulation-inputs.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plima/dev/genomic-surveillance-voi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367237C3-5CEF-C146-B9A3-29DCD4A84D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CFAAF9-D9B1-7142-B12C-38C1839BAF72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2900" yWindow="2040" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
+    <workbookView xWindow="6520" yWindow="2380" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
-    <sheet name="jurisdiction" sheetId="2" r:id="rId2"/>
-    <sheet name="travel" sheetId="3" r:id="rId3"/>
-    <sheet name="relative-mixing" sheetId="5" r:id="rId4"/>
-    <sheet name="parameters" sheetId="4" r:id="rId5"/>
+    <sheet name="parameters" sheetId="4" r:id="rId2"/>
+    <sheet name="jurisdiction" sheetId="2" r:id="rId3"/>
+    <sheet name="beta" sheetId="6" r:id="rId4"/>
+    <sheet name="travel" sheetId="3" r:id="rId5"/>
+    <sheet name="relative-mixing" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>setting</t>
   </si>
@@ -85,42 +86,21 @@
     <t>US</t>
   </si>
   <si>
-    <t>Europe</t>
-  </si>
-  <si>
     <t>NY</t>
   </si>
   <si>
     <t>NJ</t>
   </si>
   <si>
-    <t>PA</t>
-  </si>
-  <si>
-    <t>Germany</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>Italy</t>
-  </si>
-  <si>
     <t>population</t>
   </si>
   <si>
     <t>parameter</t>
   </si>
   <si>
-    <t>beta</t>
-  </si>
-  <si>
     <t>gamma</t>
   </si>
   <si>
-    <t>mean</t>
-  </si>
-  <si>
     <t>min</t>
   </si>
   <si>
@@ -133,10 +113,31 @@
     <t>jurisdiction</t>
   </si>
   <si>
-    <t>…</t>
-  </si>
-  <si>
     <t>source</t>
+  </si>
+  <si>
+    <t>sigma</t>
+  </si>
+  <si>
+    <t>baseline</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>tau</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>obs_lag</t>
+  </si>
+  <si>
+    <t>days_to_adjust_NPI</t>
   </si>
 </sst>
 </file>
@@ -505,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D12AAEB-4DB6-F84A-A5FA-6A348965EB1E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView zoomScale="181" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -524,7 +525,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -533,11 +534,112 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930774C7-2D37-094A-A2DB-7EC2D5ACBFA8}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <f>1/6</f>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <f>1/6</f>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1192CD30-F114-BB47-AF6C-7BCFE754F543}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView zoomScale="187" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D1" sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -558,7 +660,7 @@
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -566,7 +668,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -580,68 +682,12 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7">
         <v>100000</v>
       </c>
     </row>
@@ -650,19 +696,70 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D10A5E8-0BB5-4C43-827E-A5AF4D063B7C}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="str" cm="1">
+        <f t="array" ref="B1:C1">TRANSPOSE(A2:A3)</f>
+        <v>NY</v>
+      </c>
+      <c r="C1" t="str">
+        <v>NJ</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>jurisdiction!B2</f>
+        <v>NY</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>jurisdiction!B3</f>
+        <v>NJ</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A40C96AD-7FCE-D24F-B326-0D5D7D33F358}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D1" sqref="D1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B1" t="str" cm="1">
         <f t="array" ref="B1:G1">TRANSPOSE(A2:A7)</f>
@@ -671,17 +768,17 @@
       <c r="C1" t="str">
         <v>NJ</v>
       </c>
-      <c r="D1" t="str">
-        <v>PA</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Germany</v>
-      </c>
-      <c r="F1" t="str">
-        <v>France</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Italy</v>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
+      </c>
+      <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -733,9 +830,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="str">
+      <c r="A4">
         <f>jurisdiction!B4</f>
-        <v>PA</v>
+        <v>0</v>
       </c>
       <c r="B4">
         <v>0.01</v>
@@ -757,9 +854,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="str">
+      <c r="A5">
         <f>jurisdiction!B5</f>
-        <v>Germany</v>
+        <v>0</v>
       </c>
       <c r="B5">
         <v>0.01</v>
@@ -781,9 +878,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="str">
+      <c r="A6">
         <f>jurisdiction!B6</f>
-        <v>France</v>
+        <v>0</v>
       </c>
       <c r="B6">
         <v>0.01</v>
@@ -805,9 +902,9 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="str">
+      <c r="A7">
         <f>jurisdiction!B7</f>
-        <v>Italy</v>
+        <v>0</v>
       </c>
       <c r="B7">
         <v>0.01</v>
@@ -833,19 +930,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578CC606-5086-1F48-9D1A-C2900FAE3B19}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B1" t="str" cm="1">
         <f t="array" ref="B1:G1">TRANSPOSE(A2:A7)</f>
@@ -854,17 +951,17 @@
       <c r="C1" t="str">
         <v>NJ</v>
       </c>
-      <c r="D1" t="str">
-        <v>PA</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Germany</v>
-      </c>
-      <c r="F1" t="str">
-        <v>France</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Italy</v>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
+      </c>
+      <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -916,9 +1013,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="str">
+      <c r="A4">
         <f>jurisdiction!B4</f>
-        <v>PA</v>
+        <v>0</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -940,9 +1037,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="str">
+      <c r="A5">
         <f>jurisdiction!B5</f>
-        <v>Germany</v>
+        <v>0</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
@@ -964,9 +1061,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="str">
+      <c r="A6">
         <f>jurisdiction!B6</f>
-        <v>France</v>
+        <v>0</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -988,9 +1085,9 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="str">
+      <c r="A7">
         <f>jurisdiction!B7</f>
-        <v>Italy</v>
+        <v>0</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
@@ -1009,56 +1106,6 @@
       </c>
       <c r="G7" s="1">
         <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930774C7-2D37-094A-A2DB-7EC2D5ACBFA8}">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add annotations for the descriptions of variables in the metapopulation-inputs file
</commit_message>
<xml_diff>
--- a/data/metapopulation-inputs.xlsx
+++ b/data/metapopulation-inputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plima/dev/genomic-surveillance-voi/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahk/Documents/GitRepos/genomic-surveillance-voi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CFAAF9-D9B1-7142-B12C-38C1839BAF72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FCFB54-F057-6148-80F2-DB7A2652BEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6520" yWindow="2380" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
+    <workbookView xWindow="2200" yWindow="760" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>setting</t>
   </si>
@@ -138,6 +138,18 @@
   </si>
   <si>
     <t>days_to_adjust_NPI</t>
+  </si>
+  <si>
+    <t>rate of becoming symptomatic per unit time</t>
+  </si>
+  <si>
+    <t>rate of transition (exposed to pre-symptomatic)</t>
+  </si>
+  <si>
+    <t>Recovery rate per unit time</t>
+  </si>
+  <si>
+    <t>reduction in contact rate</t>
   </si>
 </sst>
 </file>
@@ -538,7 +550,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -578,6 +590,9 @@
         <f>1/6</f>
         <v>0.16666666666666666</v>
       </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -587,6 +602,9 @@
         <f>1/6</f>
         <v>0.16666666666666666</v>
       </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -596,6 +614,9 @@
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -603,6 +624,15 @@
       </c>
       <c r="B5">
         <v>0.15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -639,7 +669,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView zoomScale="187" workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -752,7 +782,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:G1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updating model, sample post-processing function
</commit_message>
<xml_diff>
--- a/data/metapopulation-inputs.xlsx
+++ b/data/metapopulation-inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plima/dev/genomic-surveillance-voi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CFAAF9-D9B1-7142-B12C-38C1839BAF72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BD2D14-BFD5-8C4C-AE1F-3FE2587924B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6520" yWindow="2380" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
+    <workbookView xWindow="-17080" yWindow="-17440" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>setting</t>
   </si>
@@ -138,13 +138,44 @@
   </si>
   <si>
     <t>days_to_adjust_NPI</t>
+  </si>
+  <si>
+    <t>cost.npi</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>infection fatality rate</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>cost of death for the average person who dies from the disease.</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>other costs of infection</t>
+  </si>
+  <si>
+    <t>C_surv</t>
+  </si>
+  <si>
+    <t>Cost of surveillance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -155,6 +186,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -183,15 +221,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -535,16 +578,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930774C7-2D37-094A-A2DB-7EC2D5ACBFA8}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -627,6 +671,51 @@
       </c>
       <c r="B8">
         <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="5">
+        <f>35*10^5</f>
+        <v>3500000</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="4">
+        <v>5000</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -636,10 +725,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1192CD30-F114-BB47-AF6C-7BCFE754F543}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView zoomScale="187" workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D8"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -647,9 +736,10 @@
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -662,8 +752,11 @@
       <c r="D1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -676,8 +769,11 @@
       <c r="D2">
         <v>100000</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="4">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -688,6 +784,9 @@
         <v>6</v>
       </c>
       <c r="D3">
+        <v>100000</v>
+      </c>
+      <c r="E3" s="4">
         <v>100000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto populate beta and travel matrices based on the jurisdiction tab. Please change the jurisdiction tab first now
</commit_message>
<xml_diff>
--- a/data/metapopulation-inputs.xlsx
+++ b/data/metapopulation-inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahk/Documents/GitRepos/genomic-surveillance-voi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD9F8AF-D0DE-D44E-A087-693FE1BC50A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECE9CE2-4419-CE4E-91B8-86C9315D1838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7720" yWindow="760" windowWidth="22400" windowHeight="17360" activeTab="4" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
+    <workbookView xWindow="7720" yWindow="760" windowWidth="22400" windowHeight="17360" activeTab="2" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -225,14 +225,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -728,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1192CD30-F114-BB47-AF6C-7BCFE754F543}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView zoomScale="187" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="187" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -892,16 +891,13 @@
   <dimension ref="A1:T54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="6"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" t="s">
         <v>15</v>
       </c>
       <c r="B1" t="str" cm="1">
@@ -964,7 +960,7 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="str">
+      <c r="A2" t="str">
         <f>IF(jurisdiction!B2="", "", jurisdiction!B2)</f>
         <v>NY</v>
       </c>
@@ -1030,7 +1026,7 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="str">
+      <c r="A3" t="str">
         <f>IF(jurisdiction!B3="", "", jurisdiction!B3)</f>
         <v>NJ</v>
       </c>
@@ -1096,7 +1092,7 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="str">
+      <c r="A4" t="str">
         <f>IF(jurisdiction!B4="", "", jurisdiction!B4)</f>
         <v/>
       </c>
@@ -1162,7 +1158,7 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="str">
+      <c r="A5" t="str">
         <f>IF(jurisdiction!B5="", "", jurisdiction!B5)</f>
         <v/>
       </c>
@@ -1228,7 +1224,7 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="str">
+      <c r="A6" t="str">
         <f>IF(jurisdiction!B6="", "", jurisdiction!B6)</f>
         <v/>
       </c>
@@ -1294,7 +1290,7 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="str">
+      <c r="A7" t="str">
         <f>IF(jurisdiction!B7="", "", jurisdiction!B7)</f>
         <v/>
       </c>
@@ -1360,7 +1356,7 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="str">
+      <c r="A8" t="str">
         <f>IF(jurisdiction!B8="", "", jurisdiction!B8)</f>
         <v/>
       </c>
@@ -1426,7 +1422,7 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="str">
+      <c r="A9" t="str">
         <f>IF(jurisdiction!B9="", "", jurisdiction!B9)</f>
         <v/>
       </c>
@@ -1492,7 +1488,7 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="str">
+      <c r="A10" t="str">
         <f>IF(jurisdiction!B10="", "", jurisdiction!B10)</f>
         <v/>
       </c>
@@ -1558,7 +1554,7 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="str">
+      <c r="A11" t="str">
         <f>IF(jurisdiction!B11="", "", jurisdiction!B11)</f>
         <v/>
       </c>
@@ -1624,7 +1620,7 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="str">
+      <c r="A12" t="str">
         <f>IF(jurisdiction!B12="", "", jurisdiction!B12)</f>
         <v/>
       </c>
@@ -1690,7 +1686,7 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="str">
+      <c r="A13" t="str">
         <f>IF(jurisdiction!B13="", "", jurisdiction!B13)</f>
         <v/>
       </c>
@@ -1756,7 +1752,7 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="str">
+      <c r="A14" t="str">
         <f>IF(jurisdiction!B14="", "", jurisdiction!B14)</f>
         <v/>
       </c>
@@ -1822,7 +1818,7 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="str">
+      <c r="A15" t="str">
         <f>IF(jurisdiction!B15="", "", jurisdiction!B15)</f>
         <v/>
       </c>
@@ -1888,7 +1884,7 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="str">
+      <c r="A16" t="str">
         <f>IF(jurisdiction!B16="", "", jurisdiction!B16)</f>
         <v/>
       </c>
@@ -1954,7 +1950,7 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="str">
+      <c r="A17" t="str">
         <f>IF(jurisdiction!B17="", "", jurisdiction!B17)</f>
         <v/>
       </c>
@@ -2020,7 +2016,7 @@
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="str">
+      <c r="A18" t="str">
         <f>IF(jurisdiction!B18="", "", jurisdiction!B18)</f>
         <v/>
       </c>
@@ -2086,7 +2082,7 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="str">
+      <c r="A19" t="str">
         <f>IF(jurisdiction!B19="", "", jurisdiction!B19)</f>
         <v/>
       </c>
@@ -2147,12 +2143,12 @@
         <v/>
       </c>
       <c r="P19" t="str">
-        <f t="shared" ref="B19:P34" si="4">IF(AND($A19&lt;&gt;"", P$1&lt;&gt;""),IF(ROW(P19)&lt;&gt;COLUMN(P19),0,1), "")</f>
+        <f t="shared" ref="P19:P34" si="4">IF(AND($A19&lt;&gt;"", P$1&lt;&gt;""),IF(ROW(P19)&lt;&gt;COLUMN(P19),0,1), "")</f>
         <v/>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="str">
+      <c r="A20" t="str">
         <f>IF(jurisdiction!B20="", "", jurisdiction!B20)</f>
         <v/>
       </c>
@@ -2218,7 +2214,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="str">
+      <c r="A21" t="str">
         <f>IF(jurisdiction!B21="", "", jurisdiction!B21)</f>
         <v/>
       </c>
@@ -2284,7 +2280,7 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="str">
+      <c r="A22" t="str">
         <f>IF(jurisdiction!B22="", "", jurisdiction!B22)</f>
         <v/>
       </c>
@@ -2350,7 +2346,7 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="str">
+      <c r="A23" t="str">
         <f>IF(jurisdiction!B23="", "", jurisdiction!B23)</f>
         <v/>
       </c>
@@ -2416,7 +2412,7 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="str">
+      <c r="A24" t="str">
         <f>IF(jurisdiction!B24="", "", jurisdiction!B24)</f>
         <v/>
       </c>
@@ -2482,7 +2478,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="str">
+      <c r="A25" t="str">
         <f>IF(jurisdiction!B25="", "", jurisdiction!B25)</f>
         <v/>
       </c>
@@ -2548,7 +2544,7 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="str">
+      <c r="A26" t="str">
         <f>IF(jurisdiction!B26="", "", jurisdiction!B26)</f>
         <v/>
       </c>
@@ -2614,7 +2610,7 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="str">
+      <c r="A27" t="str">
         <f>IF(jurisdiction!B27="", "", jurisdiction!B27)</f>
         <v/>
       </c>
@@ -2680,7 +2676,7 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="str">
+      <c r="A28" t="str">
         <f>IF(jurisdiction!B28="", "", jurisdiction!B28)</f>
         <v/>
       </c>
@@ -2746,7 +2742,7 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="str">
+      <c r="A29" t="str">
         <f>IF(jurisdiction!B29="", "", jurisdiction!B29)</f>
         <v/>
       </c>
@@ -2812,7 +2808,7 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="str">
+      <c r="A30" t="str">
         <f>IF(jurisdiction!B30="", "", jurisdiction!B30)</f>
         <v/>
       </c>
@@ -2878,7 +2874,7 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="str">
+      <c r="A31" t="str">
         <f>IF(jurisdiction!B31="", "", jurisdiction!B31)</f>
         <v/>
       </c>
@@ -2944,7 +2940,7 @@
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="str">
+      <c r="A32" t="str">
         <f>IF(jurisdiction!B32="", "", jurisdiction!B32)</f>
         <v/>
       </c>
@@ -3010,7 +3006,7 @@
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="str">
+      <c r="A33" t="str">
         <f>IF(jurisdiction!B33="", "", jurisdiction!B33)</f>
         <v/>
       </c>
@@ -3076,7 +3072,7 @@
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="str">
+      <c r="A34" t="str">
         <f>IF(jurisdiction!B34="", "", jurisdiction!B34)</f>
         <v/>
       </c>
@@ -3142,7 +3138,7 @@
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A35" s="6" t="str">
+      <c r="A35" t="str">
         <f>IF(jurisdiction!B35="", "", jurisdiction!B35)</f>
         <v/>
       </c>
@@ -3203,12 +3199,12 @@
         <v/>
       </c>
       <c r="P35" t="str">
-        <f t="shared" ref="B35:P35" si="5">IF(AND($A35&lt;&gt;"", P$1&lt;&gt;""),IF(ROW(P35)&lt;&gt;COLUMN(P35),0,1), "")</f>
+        <f t="shared" ref="P35" si="5">IF(AND($A35&lt;&gt;"", P$1&lt;&gt;""),IF(ROW(P35)&lt;&gt;COLUMN(P35),0,1), "")</f>
         <v/>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="str">
+      <c r="A36" t="str">
         <f>IF(jurisdiction!B36="", "", jurisdiction!B36)</f>
         <v/>
       </c>
@@ -3270,7 +3266,7 @@
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="str">
+      <c r="A37" t="str">
         <f>IF(jurisdiction!B37="", "", jurisdiction!B37)</f>
         <v/>
       </c>
@@ -3332,7 +3328,7 @@
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A38" s="6" t="str">
+      <c r="A38" t="str">
         <f>IF(jurisdiction!B38="", "", jurisdiction!B38)</f>
         <v/>
       </c>
@@ -3394,7 +3390,7 @@
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A39" s="6" t="str">
+      <c r="A39" t="str">
         <f>IF(jurisdiction!B39="", "", jurisdiction!B39)</f>
         <v/>
       </c>
@@ -3456,7 +3452,7 @@
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A40" s="6" t="str">
+      <c r="A40" t="str">
         <f>IF(jurisdiction!B40="", "", jurisdiction!B40)</f>
         <v/>
       </c>
@@ -3518,7 +3514,7 @@
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A41" s="6" t="str">
+      <c r="A41" t="str">
         <f>IF(jurisdiction!B41="", "", jurisdiction!B41)</f>
         <v/>
       </c>
@@ -4342,8 +4338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A40C96AD-7FCE-D24F-B326-0D5D7D33F358}">
   <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
move nr_patches to parameters for now, and read in from that file, rather than hard coding
</commit_message>
<xml_diff>
--- a/data/metapopulation-inputs.xlsx
+++ b/data/metapopulation-inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahk/Documents/GitRepos/genomic-surveillance-voi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECE9CE2-4419-CE4E-91B8-86C9315D1838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F5E7E8-E987-4E49-9714-5B6812524FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7720" yWindow="760" windowWidth="22400" windowHeight="17360" activeTab="2" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
+    <workbookView xWindow="7720" yWindow="760" windowWidth="22400" windowHeight="17360" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -549,7 +549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D12AAEB-4DB6-F84A-A5FA-6A348965EB1E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScale="181" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="181" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -568,7 +568,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -578,10 +578,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930774C7-2D37-094A-A2DB-7EC2D5ACBFA8}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScale="141" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -718,6 +718,16 @@
         <v>33</v>
       </c>
     </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="str">
+        <f>settings!A2</f>
+        <v>nr_patches</v>
+      </c>
+      <c r="B13">
+        <f>settings!B2</f>
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -727,7 +737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1192CD30-F114-BB47-AF6C-7BCFE754F543}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="187" workbookViewId="0">
+    <sheetView zoomScale="187" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Name parameters within excel sheet so that they can be used elsewhere in the excel document without having to do a location reference
</commit_message>
<xml_diff>
--- a/data/metapopulation-inputs.xlsx
+++ b/data/metapopulation-inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahk/Documents/GitRepos/genomic-surveillance-voi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F5E7E8-E987-4E49-9714-5B6812524FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A468269C-86A4-064C-B44F-7D939288B9AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7720" yWindow="760" windowWidth="22400" windowHeight="17360" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
+    <workbookView xWindow="7720" yWindow="760" windowWidth="22400" windowHeight="17360" activeTab="1" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,20 @@
     <sheet name="travel" sheetId="3" r:id="rId5"/>
     <sheet name="relative-mixing" sheetId="5" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="c_">parameters!$B$6</definedName>
+    <definedName name="C_surv">parameters!$B$12</definedName>
+    <definedName name="days_to_adjust_NPI">parameters!$B$8</definedName>
+    <definedName name="delta">parameters!$B$3</definedName>
+    <definedName name="gamma">parameters!$B$4</definedName>
+    <definedName name="nr_patches">parameters!$B$13</definedName>
+    <definedName name="o">parameters!$B$11</definedName>
+    <definedName name="obs_lag">parameters!$B$7</definedName>
+    <definedName name="r_">parameters!$B$9</definedName>
+    <definedName name="sigma">parameters!$B$2</definedName>
+    <definedName name="tau">parameters!$B$5</definedName>
+    <definedName name="w">parameters!$B$10</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -549,7 +563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D12AAEB-4DB6-F84A-A5FA-6A348965EB1E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="181" workbookViewId="0">
+    <sheetView zoomScale="181" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -580,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930774C7-2D37-094A-A2DB-7EC2D5ACBFA8}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView zoomScale="141" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -901,7 +915,7 @@
   <dimension ref="A1:T54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Read in nr_patches directly from the settings tab so as to avoid accidentally forgetting to update it
</commit_message>
<xml_diff>
--- a/data/metapopulation-inputs.xlsx
+++ b/data/metapopulation-inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahk/Documents/GitRepos/genomic-surveillance-voi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A468269C-86A4-064C-B44F-7D939288B9AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4E95C6-946A-7B4D-B1D3-75F9B98FC1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7720" yWindow="760" windowWidth="22400" windowHeight="17360" activeTab="1" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
+    <workbookView xWindow="6820" yWindow="760" windowWidth="22400" windowHeight="17180" activeTab="1" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -592,10 +592,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930774C7-2D37-094A-A2DB-7EC2D5ACBFA8}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -730,16 +730,6 @@
       </c>
       <c r="C12" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="str">
-        <f>settings!A2</f>
-        <v>nr_patches</v>
-      </c>
-      <c r="B13">
-        <f>settings!B2</f>
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Support auto-population of multiple patches
</commit_message>
<xml_diff>
--- a/data/metapopulation-inputs.xlsx
+++ b/data/metapopulation-inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahk/Documents/GitRepos/genomic-surveillance-voi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4E95C6-946A-7B4D-B1D3-75F9B98FC1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB49C7D-C7E2-8B45-9826-BEBC2A96235C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6820" yWindow="760" windowWidth="22400" windowHeight="17180" activeTab="1" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
+    <workbookView xWindow="7840" yWindow="760" windowWidth="22400" windowHeight="17180" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>setting</t>
   </si>
@@ -179,6 +179,15 @@
   </si>
   <si>
     <t>Cost of surveillance</t>
+  </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t>bar</t>
+  </si>
+  <si>
+    <t>PA</t>
   </si>
 </sst>
 </file>
@@ -561,9 +570,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D12AAEB-4DB6-F84A-A5FA-6A348965EB1E}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView zoomScale="181" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="181" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -582,7 +591,16 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <f>MAX(jurisdiction!A:A)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -594,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930774C7-2D37-094A-A2DB-7EC2D5ACBFA8}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView zoomScale="141" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -742,7 +760,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView zoomScale="187" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -802,7 +820,24 @@
         <v>100000</v>
       </c>
       <c r="E3" s="4">
-        <v>100000</v>
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>200000</v>
+      </c>
+      <c r="E4">
+        <v>200000</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -922,7 +957,7 @@
         <v>NJ</v>
       </c>
       <c r="D1" t="str">
-        <v/>
+        <v>PA</v>
       </c>
       <c r="E1" t="str">
         <v/>
@@ -986,9 +1021,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D2" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="D2">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="E2" t="str">
         <f t="shared" si="0"/>
@@ -1052,9 +1087,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="D3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" si="0"/>
@@ -1108,19 +1143,19 @@
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>IF(jurisdiction!B4="", "", jurisdiction!B4)</f>
-        <v/>
-      </c>
-      <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <v>PA</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
@@ -4373,7 +4408,7 @@
       </c>
       <c r="D1" t="str">
         <f>beta!D1</f>
-        <v/>
+        <v>PA</v>
       </c>
       <c r="E1" t="str">
         <f>beta!E1</f>
@@ -4437,9 +4472,9 @@
         <f t="shared" ref="C2:L2" si="0">IF(OR($A2="", C$1=""), "", IF(ROW(C2)=COLUMN(C2),-0.05,0.01))</f>
         <v>0.01</v>
       </c>
-      <c r="D2" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="D2">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
       </c>
       <c r="E2" t="str">
         <f t="shared" si="0"/>
@@ -4487,9 +4522,9 @@
         <f t="shared" si="1"/>
         <v>-0.05</v>
       </c>
-      <c r="D3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="D3">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" si="1"/>
@@ -4527,19 +4562,19 @@
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>IF(beta!A4="","",beta!A4)</f>
-        <v/>
-      </c>
-      <c r="B4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="D4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>PA</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>-0.05</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="1"/>
@@ -6022,8 +6057,8 @@
       <c r="C1" t="str">
         <v>NJ</v>
       </c>
-      <c r="D1">
-        <v>0</v>
+      <c r="D1" t="str">
+        <v>PA</v>
       </c>
       <c r="E1">
         <v>0</v>
@@ -6084,9 +6119,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" t="str">
         <f>jurisdiction!B4</f>
-        <v>0</v>
+        <v>PA</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>

</xml_diff>